<commit_message>
Signed-off-by: Arun Ganesh Alagappan <arunganesha@Mav.Est>
</commit_message>
<xml_diff>
--- a/DataBase/TestDataDB/TestData.xlsx
+++ b/DataBase/TestDataDB/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235" tabRatio="829"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="829"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t>https://www.google.co.in/</t>
   </si>
   <si>
-    <t>chrome</t>
+    <t>firefox</t>
   </si>
 </sst>
 </file>

</xml_diff>